<commit_message>
Vygenerovany vysledky rozmistovani svitidel pro dfinovanou krivku svitivosti.
</commit_message>
<xml_diff>
--- a/LightSvetlo2015/GASVP_test1/nastaveni a vysledky.xlsx
+++ b/LightSvetlo2015/GASVP_test1/nastaveni a vysledky.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -188,15 +188,9 @@
     <t>Fitness:</t>
   </si>
   <si>
-    <t>pop.FIT = (1 + ((10*(target.Uo-pop.Uo)).^2) + pop.sym + (0.1*(pop.Eavg-target.Eavg)).^2).*pop.dna(:,(2*svt.N)+1);</t>
-  </si>
-  <si>
     <t>Nastavení:</t>
   </si>
   <si>
-    <t xml:space="preserve">                pop.gen = 150;</t>
-  </si>
-  <si>
     <t>DNA</t>
   </si>
   <si>
@@ -252,6 +246,12 @@
   </si>
   <si>
     <t>Fitness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                pop.gen = 100;</t>
+  </si>
+  <si>
+    <t>pop.FIT = (((10*(target.Uo-pop.Uo)).^2) + pop.var + (0.1*(pop.Eavg-target.Eavg)).^2);</t>
   </si>
 </sst>
 </file>
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
   <a:themeElements>
     <a:clrScheme name="Kancelář">
       <a:dk1>
@@ -372,7 +372,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kancelář">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -407,7 +407,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -619,7 +619,7 @@
   <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>56</v>
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CV22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,7 +966,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -983,1038 +983,1038 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>1.3844725010363199</v>
+        <v>0.84750600561667999</v>
       </c>
       <c r="B3" s="4">
-        <v>5</v>
+        <v>3.7368091224538902</v>
       </c>
       <c r="C3" s="4">
-        <v>4.4638504529230998</v>
+        <v>4.53384817935875</v>
       </c>
       <c r="D3" s="4">
-        <v>2.9958016736808299</v>
+        <v>4.7220084179142496</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>5.0078775589250197</v>
       </c>
       <c r="F3" s="4">
-        <v>0.93312989788163403</v>
+        <v>1.18295113381124</v>
       </c>
       <c r="G3" s="4">
-        <v>10</v>
+        <v>8.4495301578468496</v>
       </c>
       <c r="H3" s="4">
-        <v>4.2171675508721904</v>
+        <v>4.0062531007423798</v>
       </c>
       <c r="I3" s="4">
-        <v>5.6136684898403804</v>
+        <v>8.4704251933810504</v>
       </c>
       <c r="J3" s="4">
-        <v>1.9582027703210101</v>
+        <v>1.0833240375011299</v>
       </c>
       <c r="K3" s="4">
-        <v>8.6959596091878506</v>
+        <v>1.73413239625997</v>
       </c>
       <c r="L3" s="4">
-        <v>0</v>
+        <v>0.61967313801601798</v>
       </c>
       <c r="M3" s="4">
-        <v>6300.0671493173304</v>
+        <v>5544.1957030636304</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B7" s="4">
         <v>0.5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8" s="4">
         <v>0.25</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>404.28482518617</v>
+        <v>285.16849647032001</v>
       </c>
       <c r="B10" s="4">
-        <v>399.46546566073999</v>
+        <v>483.05317766744201</v>
       </c>
       <c r="C10" s="4">
-        <v>370.31960864635698</v>
+        <v>698.95502398593999</v>
       </c>
       <c r="D10" s="4">
-        <v>334.588985958889</v>
+        <v>799.23363773707001</v>
       </c>
       <c r="E10" s="4">
-        <v>307.44642499610597</v>
+        <v>703.86828290376798</v>
       </c>
       <c r="F10" s="4">
-        <v>296.74761061005597</v>
+        <v>514.37624866950603</v>
       </c>
       <c r="G10" s="4">
-        <v>303.71791119349598</v>
+        <v>382.83711629002698</v>
       </c>
       <c r="H10" s="4">
-        <v>325.10739138996303</v>
+        <v>371.49798548648403</v>
       </c>
       <c r="I10" s="4">
-        <v>354.76483280324601</v>
+        <v>453.42458615887602</v>
       </c>
       <c r="J10" s="4">
-        <v>384.991189594378</v>
+        <v>540.39038179534998</v>
       </c>
       <c r="K10" s="4">
-        <v>408.84724447759601</v>
+        <v>537.61127050537095</v>
       </c>
       <c r="L10" s="4">
-        <v>423.56099801527301</v>
+        <v>439.94562728071401</v>
       </c>
       <c r="M10" s="4">
-        <v>432.87929661811</v>
+        <v>332.497709026645</v>
       </c>
       <c r="N10" s="4">
-        <v>445.13290824081503</v>
+        <v>294.090403894855</v>
       </c>
       <c r="O10" s="4">
-        <v>466.43423730870597</v>
+        <v>351.06632587215103</v>
       </c>
       <c r="P10" s="4">
-        <v>493.16021310758998</v>
+        <v>475.710056419083</v>
       </c>
       <c r="Q10" s="4">
-        <v>510.31356485157397</v>
+        <v>579.41885769219402</v>
       </c>
       <c r="R10" s="4">
-        <v>499.397093339702</v>
+        <v>565.57576787564096</v>
       </c>
       <c r="S10" s="4">
-        <v>451.17528935801499</v>
+        <v>438.00588126046</v>
       </c>
       <c r="T10" s="4">
-        <v>372.645777398902</v>
+        <v>281.61021556212302</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>463.388487975224</v>
+        <v>317.78772702964199</v>
       </c>
       <c r="B11" s="4">
-        <v>460.214442438015</v>
+        <v>532.36945906774201</v>
       </c>
       <c r="C11" s="4">
-        <v>429.80021144339202</v>
+        <v>764.08892505076403</v>
       </c>
       <c r="D11" s="4">
-        <v>393.07570170373498</v>
+        <v>871.07081057504297</v>
       </c>
       <c r="E11" s="4">
-        <v>368.01300941616603</v>
+        <v>768.40047740505304</v>
       </c>
       <c r="F11" s="4">
-        <v>363.99127098009598</v>
+        <v>569.34704441132703</v>
       </c>
       <c r="G11" s="4">
-        <v>382.35520143290699</v>
+        <v>444.13067871559298</v>
       </c>
       <c r="H11" s="4">
-        <v>418.49944077449197</v>
+        <v>468.15464985125499</v>
       </c>
       <c r="I11" s="4">
-        <v>463.38222484756801</v>
+        <v>613.67690887165895</v>
       </c>
       <c r="J11" s="4">
-        <v>505.20515293202197</v>
+        <v>758.72851636555299</v>
       </c>
       <c r="K11" s="4">
-        <v>532.80301545233499</v>
+        <v>757.41474124797196</v>
       </c>
       <c r="L11" s="4">
-        <v>540.85726672594001</v>
+        <v>604.32637850137701</v>
       </c>
       <c r="M11" s="4">
-        <v>533.78131742210496</v>
+        <v>437.62653941690701</v>
       </c>
       <c r="N11" s="4">
-        <v>523.57303536658003</v>
+        <v>375.884208190202</v>
       </c>
       <c r="O11" s="4">
-        <v>521.113242820849</v>
+        <v>454.54514503070698</v>
       </c>
       <c r="P11" s="4">
-        <v>526.92330995268799</v>
+        <v>635.19652337495904</v>
       </c>
       <c r="Q11" s="4">
-        <v>528.97372460834595</v>
+        <v>789.43299845428999</v>
       </c>
       <c r="R11" s="4">
-        <v>510.19084131798002</v>
+        <v>770.62385039471098</v>
       </c>
       <c r="S11" s="4">
-        <v>460.45826531498699</v>
+        <v>585.65624597975204</v>
       </c>
       <c r="T11" s="4">
-        <v>383.79171730166701</v>
+        <v>365.26153872444598</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>482.85304797928802</v>
+        <v>302.98830650975299</v>
       </c>
       <c r="B12" s="4">
-        <v>485.97177650114298</v>
+        <v>477.876291016994</v>
       </c>
       <c r="C12" s="4">
-        <v>462.40973129813602</v>
+        <v>654.31495149772695</v>
       </c>
       <c r="D12" s="4">
-        <v>433.41751973910999</v>
+        <v>731.05013701573102</v>
       </c>
       <c r="E12" s="4">
-        <v>417.93882771768102</v>
+        <v>652.02767294058106</v>
       </c>
       <c r="F12" s="4">
-        <v>426.447797176937</v>
+        <v>505.84976935419797</v>
       </c>
       <c r="G12" s="4">
-        <v>460.58954946198799</v>
+        <v>427.72723718638002</v>
       </c>
       <c r="H12" s="4">
-        <v>514.36216877963204</v>
+        <v>487.40532233717101</v>
       </c>
       <c r="I12" s="4">
-        <v>575.38630885199996</v>
+        <v>665.01551154312403</v>
       </c>
       <c r="J12" s="4">
-        <v>627.38220445059903</v>
+        <v>834.44618137381894</v>
       </c>
       <c r="K12" s="4">
-        <v>655.16202987168799</v>
+        <v>834.45017075442695</v>
       </c>
       <c r="L12" s="4">
-        <v>651.630229567377</v>
+        <v>661.12782759178697</v>
       </c>
       <c r="M12" s="4">
-        <v>622.73802202482295</v>
+        <v>472.91282702115802</v>
       </c>
       <c r="N12" s="4">
-        <v>584.74558000534796</v>
+        <v>401.20632682813698</v>
       </c>
       <c r="O12" s="4">
-        <v>553.68463022668698</v>
+        <v>481.97724274599898</v>
       </c>
       <c r="P12" s="4">
-        <v>534.80166562501404</v>
+        <v>672.61293744919203</v>
       </c>
       <c r="Q12" s="4">
-        <v>520.03111298360704</v>
+        <v>836.12130952257496</v>
       </c>
       <c r="R12" s="4">
-        <v>494.68392458098901</v>
+        <v>815.965316867703</v>
       </c>
       <c r="S12" s="4">
-        <v>447.865844712566</v>
+        <v>619.43770891486099</v>
       </c>
       <c r="T12" s="4">
-        <v>379.47470550594102</v>
+        <v>386.13446135644</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>466.41906370173302</v>
+        <v>291.12470139216703</v>
       </c>
       <c r="B13" s="4">
-        <v>480.411812107267</v>
+        <v>411.76415841364502</v>
       </c>
       <c r="C13" s="4">
-        <v>470.99635694671701</v>
+        <v>509.164446098545</v>
       </c>
       <c r="D13" s="4">
-        <v>456.92917921601997</v>
+        <v>537.39510977371503</v>
       </c>
       <c r="E13" s="4">
-        <v>456.35627740219599</v>
+        <v>480.585469518004</v>
       </c>
       <c r="F13" s="4">
-        <v>480.43323849224902</v>
+        <v>395.59290891464201</v>
       </c>
       <c r="G13" s="4">
-        <v>531.26431230131402</v>
+        <v>363.30755206189502</v>
       </c>
       <c r="H13" s="4">
-        <v>601.40209585637604</v>
+        <v>429.93310134056799</v>
       </c>
       <c r="I13" s="4">
-        <v>674.898580850548</v>
+        <v>580.10521297164598</v>
       </c>
       <c r="J13" s="4">
-        <v>731.41799795489999</v>
+        <v>716.17115354167595</v>
       </c>
       <c r="K13" s="4">
-        <v>753.45479699842599</v>
+        <v>715.60978084775797</v>
       </c>
       <c r="L13" s="4">
-        <v>734.42223202851301</v>
+        <v>577.681969322339</v>
       </c>
       <c r="M13" s="4">
-        <v>683.13820776181694</v>
+        <v>427.19037355072697</v>
       </c>
       <c r="N13" s="4">
-        <v>619.80197743434098</v>
+        <v>370.33530793160003</v>
       </c>
       <c r="O13" s="4">
-        <v>564.35860879331995</v>
+        <v>436.043773567686</v>
       </c>
       <c r="P13" s="4">
-        <v>525.70023265456905</v>
+        <v>586.20847131446499</v>
       </c>
       <c r="Q13" s="4">
-        <v>499.15460670900302</v>
+        <v>711.531880563968</v>
       </c>
       <c r="R13" s="4">
-        <v>472.103849916576</v>
+        <v>694.16018507925105</v>
       </c>
       <c r="S13" s="4">
-        <v>432.56695368080602</v>
+        <v>538.73770759194895</v>
       </c>
       <c r="T13" s="4">
-        <v>375.94628670416199</v>
+        <v>347.39615233908302</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>432.35412291890299</v>
+        <v>338.615433542262</v>
       </c>
       <c r="B14" s="4">
-        <v>460.05430502975798</v>
+        <v>431.10609495030297</v>
       </c>
       <c r="C14" s="4">
-        <v>468.24112964338201</v>
+        <v>464.27734769347001</v>
       </c>
       <c r="D14" s="4">
-        <v>471.390912840086</v>
+        <v>435.953980028768</v>
       </c>
       <c r="E14" s="4">
-        <v>485.71971010077999</v>
+        <v>370.50718419317201</v>
       </c>
       <c r="F14" s="4">
-        <v>522.81003810769096</v>
+        <v>311.58116321386802</v>
       </c>
       <c r="G14" s="4">
-        <v>585.42873768798802</v>
+        <v>298.42277234044298</v>
       </c>
       <c r="H14" s="4">
-        <v>664.943248400931</v>
+        <v>348.14263611375799</v>
       </c>
       <c r="I14" s="4">
-        <v>742.33436902166795</v>
+        <v>442.67217098171102</v>
       </c>
       <c r="J14" s="4">
-        <v>794.66429206033604</v>
+        <v>520.85700351912703</v>
       </c>
       <c r="K14" s="4">
-        <v>804.80826899763497</v>
+        <v>516.29280123517105</v>
       </c>
       <c r="L14" s="4">
-        <v>769.43883057533606</v>
+        <v>433.00102771308599</v>
       </c>
       <c r="M14" s="4">
-        <v>701.09166865847305</v>
+        <v>344.86999091715097</v>
       </c>
       <c r="N14" s="4">
-        <v>622.30061487646697</v>
+        <v>318.89855018571598</v>
       </c>
       <c r="O14" s="4">
-        <v>554.25829841533903</v>
+        <v>375.05379964826102</v>
       </c>
       <c r="P14" s="4">
-        <v>507.323488906823</v>
+        <v>483.83346116288601</v>
       </c>
       <c r="Q14" s="4">
-        <v>478.87242886944301</v>
+        <v>568.84457666389403</v>
       </c>
       <c r="R14" s="4">
-        <v>457.52006856269298</v>
+        <v>554.52729779656795</v>
       </c>
       <c r="S14" s="4">
-        <v>429.73563077639801</v>
+        <v>443.73026346075102</v>
       </c>
       <c r="T14" s="4">
-        <v>386.41032944439701</v>
+        <v>299.38213915655803</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>401.15448410227702</v>
+        <v>470.36569888164303</v>
       </c>
       <c r="B15" s="4">
-        <v>443.43330857996102</v>
+        <v>573.52837582719599</v>
       </c>
       <c r="C15" s="4">
-        <v>468.44319826410498</v>
+        <v>559.02073726193203</v>
       </c>
       <c r="D15" s="4">
-        <v>485.63957493289797</v>
+        <v>459.68250352417903</v>
       </c>
       <c r="E15" s="4">
-        <v>508.89948113293599</v>
+        <v>349.730273031195</v>
       </c>
       <c r="F15" s="4">
-        <v>550.29557060901095</v>
+        <v>281.54524142698</v>
       </c>
       <c r="G15" s="4">
-        <v>613.79724924457298</v>
+        <v>270.139865559182</v>
       </c>
       <c r="H15" s="4">
-        <v>690.68393162978805</v>
+        <v>306.90311794505999</v>
       </c>
       <c r="I15" s="4">
-        <v>760.65887000259295</v>
+        <v>363.85702880257497</v>
       </c>
       <c r="J15" s="4">
-        <v>800.55865013624202</v>
+        <v>399.04007993673099</v>
       </c>
       <c r="K15" s="4">
-        <v>795.99016114960205</v>
+        <v>383.33113556819097</v>
       </c>
       <c r="L15" s="4">
-        <v>748.15964077556998</v>
+        <v>329.92120922677799</v>
       </c>
       <c r="M15" s="4">
-        <v>672.62813611324304</v>
+        <v>284.66434540314901</v>
       </c>
       <c r="N15" s="4">
-        <v>591.84153131297899</v>
+        <v>289.62509944157</v>
       </c>
       <c r="O15" s="4">
-        <v>525.44057560876104</v>
+        <v>360.11816217348098</v>
       </c>
       <c r="P15" s="4">
-        <v>483.218896239532</v>
+        <v>471.41370219435203</v>
       </c>
       <c r="Q15" s="4">
-        <v>463.44640947398102</v>
+        <v>553.944328170988</v>
       </c>
       <c r="R15" s="4">
-        <v>455.31043924242999</v>
+        <v>539.11939502597795</v>
       </c>
       <c r="S15" s="4">
-        <v>443.38547626409701</v>
+        <v>432.09917122254598</v>
       </c>
       <c r="T15" s="4">
-        <v>414.08462356185203</v>
+        <v>292.76583516409897</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>384.59919326436102</v>
+        <v>636.18936781800198</v>
       </c>
       <c r="B16" s="4">
-        <v>441.12411930119902</v>
+        <v>772.88585623251095</v>
       </c>
       <c r="C16" s="4">
-        <v>479.64197310185199</v>
+        <v>721.74876780296802</v>
       </c>
       <c r="D16" s="4">
-        <v>504.35276964097397</v>
+        <v>546.96196073806198</v>
       </c>
       <c r="E16" s="4">
-        <v>526.89193273248895</v>
+        <v>380.20389688998699</v>
       </c>
       <c r="F16" s="4">
-        <v>560.30766131551104</v>
+        <v>293.87587562452001</v>
       </c>
       <c r="G16" s="4">
-        <v>610.82306870443699</v>
+        <v>290.78562675562603</v>
       </c>
       <c r="H16" s="4">
-        <v>671.59954616170899</v>
+        <v>342.40952919070298</v>
       </c>
       <c r="I16" s="4">
-        <v>723.90402932927395</v>
+        <v>400.92198235915902</v>
       </c>
       <c r="J16" s="4">
-        <v>746.95700066300503</v>
+        <v>416.00732593556398</v>
       </c>
       <c r="K16" s="4">
-        <v>729.99463005160203</v>
+        <v>373.82073668832902</v>
       </c>
       <c r="L16" s="4">
-        <v>677.56838798939202</v>
+        <v>308.63258498714703</v>
       </c>
       <c r="M16" s="4">
-        <v>605.93201077240803</v>
+        <v>270.07784486364602</v>
       </c>
       <c r="N16" s="4">
-        <v>535.12849833600706</v>
+        <v>295.33612937619603</v>
       </c>
       <c r="O16" s="4">
-        <v>481.56163908686199</v>
+        <v>400.73382311024602</v>
       </c>
       <c r="P16" s="4">
-        <v>453.45764864169502</v>
+        <v>560.344359985898</v>
       </c>
       <c r="Q16" s="4">
-        <v>449.44896839163198</v>
+        <v>680.84153742165699</v>
       </c>
       <c r="R16" s="4">
-        <v>459.070724790008</v>
+        <v>661.19551286098601</v>
       </c>
       <c r="S16" s="4">
-        <v>465.05362375680102</v>
+        <v>513.14904624674205</v>
       </c>
       <c r="T16" s="4">
-        <v>449.64647087732999</v>
+        <v>332.61521311783201</v>
       </c>
     </row>
     <row r="17" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>381.58806354492901</v>
+        <v>710.76774586820795</v>
       </c>
       <c r="B17" s="4">
-        <v>450.93507088205303</v>
+        <v>864.67193389663498</v>
       </c>
       <c r="C17" s="4">
-        <v>498.81789285032602</v>
+        <v>797.46837670379</v>
       </c>
       <c r="D17" s="4">
-        <v>524.17607908978596</v>
+        <v>588.88942338498805</v>
       </c>
       <c r="E17" s="4">
-        <v>536.75518670822396</v>
+        <v>400.58379564018401</v>
       </c>
       <c r="F17" s="4">
-        <v>551.29422166818301</v>
+        <v>319.29070158524001</v>
       </c>
       <c r="G17" s="4">
-        <v>577.47062515315997</v>
+        <v>349.240218698886</v>
       </c>
       <c r="H17" s="4">
-        <v>612.33087778774495</v>
+        <v>453.58957577870598</v>
       </c>
       <c r="I17" s="4">
-        <v>641.30303002305095</v>
+        <v>554.866207038938</v>
       </c>
       <c r="J17" s="4">
-        <v>647.78147971064197</v>
+        <v>565.23603932027697</v>
       </c>
       <c r="K17" s="4">
-        <v>624.08986267514501</v>
+        <v>473.31062599148601</v>
       </c>
       <c r="L17" s="4">
-        <v>575.51739861885903</v>
+        <v>354.82533554223301</v>
       </c>
       <c r="M17" s="4">
-        <v>516.24538048038198</v>
+        <v>288.21885802534501</v>
       </c>
       <c r="N17" s="4">
-        <v>462.40386989188403</v>
+        <v>314.39579830925101</v>
       </c>
       <c r="O17" s="4">
-        <v>426.75782420520198</v>
+        <v>448.54183509273003</v>
       </c>
       <c r="P17" s="4">
-        <v>415.884866446736</v>
+        <v>659.43942279943406</v>
       </c>
       <c r="Q17" s="4">
-        <v>428.68663329061002</v>
+        <v>823.32651573970702</v>
       </c>
       <c r="R17" s="4">
-        <v>455.20165923326903</v>
+        <v>798.27268875055597</v>
       </c>
       <c r="S17" s="4">
-        <v>477.07119934581601</v>
+        <v>602.68902174321602</v>
       </c>
       <c r="T17" s="4">
-        <v>473.61764059607401</v>
+        <v>375.209388773142</v>
       </c>
     </row>
     <row r="18" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>380.25508082555803</v>
+        <v>619.54972336797698</v>
       </c>
       <c r="B18" s="4">
-        <v>458.79206080528201</v>
+        <v>749.54776493059103</v>
       </c>
       <c r="C18" s="4">
-        <v>511.54437400760798</v>
+        <v>693.84368948469501</v>
       </c>
       <c r="D18" s="4">
-        <v>532.69440245340195</v>
+        <v>521.81044907183696</v>
       </c>
       <c r="E18" s="4">
-        <v>530.46408326331596</v>
+        <v>371.788583453081</v>
       </c>
       <c r="F18" s="4">
-        <v>521.57197932512202</v>
+        <v>327.88062586731098</v>
       </c>
       <c r="G18" s="4">
-        <v>519.59626107666998</v>
+        <v>408.68008615698699</v>
       </c>
       <c r="H18" s="4">
-        <v>526.34736902343298</v>
+        <v>584.34227949514104</v>
       </c>
       <c r="I18" s="4">
-        <v>532.51060761662802</v>
+        <v>748.48095921601202</v>
       </c>
       <c r="J18" s="4">
-        <v>526.04196028773595</v>
+        <v>761.17517659007206</v>
       </c>
       <c r="K18" s="4">
-        <v>501.24213621170298</v>
+        <v>608.27419631965597</v>
       </c>
       <c r="L18" s="4">
-        <v>461.99609173482497</v>
+        <v>418.76063344083798</v>
       </c>
       <c r="M18" s="4">
-        <v>418.67234853283702</v>
+        <v>307.11066462795498</v>
       </c>
       <c r="N18" s="4">
-        <v>382.99026214548098</v>
+        <v>313.048188731739</v>
       </c>
       <c r="O18" s="4">
-        <v>364.35163968532999</v>
+        <v>440.02903243444399</v>
       </c>
       <c r="P18" s="4">
-        <v>367.875562425525</v>
+        <v>649.31451511628495</v>
       </c>
       <c r="Q18" s="4">
-        <v>392.68653535196597</v>
+        <v>813.42992689407004</v>
       </c>
       <c r="R18" s="4">
-        <v>429.706867943936</v>
+        <v>788.43264965394599</v>
       </c>
       <c r="S18" s="4">
-        <v>461.02195110723397</v>
+        <v>592.83887019566805</v>
       </c>
       <c r="T18" s="4">
-        <v>465.47395159865698</v>
+        <v>366.48949973073798</v>
       </c>
     </row>
     <row r="19" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>365.167442649745</v>
+        <v>428.34512896549899</v>
       </c>
       <c r="B19" s="4">
-        <v>446.13856232331602</v>
+        <v>511.29661379349</v>
       </c>
       <c r="C19" s="4">
-        <v>498.72446188593102</v>
+        <v>479.85772489658399</v>
       </c>
       <c r="D19" s="4">
-        <v>513.76565474438905</v>
+        <v>378.48487349104602</v>
       </c>
       <c r="E19" s="4">
-        <v>498.12304855283497</v>
+        <v>295.18496239961098</v>
       </c>
       <c r="F19" s="4">
-        <v>469.620025908527</v>
+        <v>295.82143203886102</v>
       </c>
       <c r="G19" s="4">
-        <v>444.633627906318</v>
+        <v>410.10096510211002</v>
       </c>
       <c r="H19" s="4">
-        <v>428.96839719778598</v>
+        <v>620.65278899723</v>
       </c>
       <c r="I19" s="4">
-        <v>418.02875322590199</v>
+        <v>814.22028035947005</v>
       </c>
       <c r="J19" s="4">
-        <v>403.67850558141402</v>
+        <v>828.67172281001001</v>
       </c>
       <c r="K19" s="4">
-        <v>381.35962095417398</v>
+        <v>648.60830954609696</v>
       </c>
       <c r="L19" s="4">
-        <v>352.838478044228</v>
+        <v>426.75445971733598</v>
       </c>
       <c r="M19" s="4">
-        <v>324.46837479340002</v>
+        <v>289.92630293603702</v>
       </c>
       <c r="N19" s="4">
-        <v>303.90754682539199</v>
+        <v>269.64901835642002</v>
       </c>
       <c r="O19" s="4">
-        <v>297.64200397692798</v>
+        <v>354.90740380468702</v>
       </c>
       <c r="P19" s="4">
-        <v>309.41055436565802</v>
+        <v>504.66289445938799</v>
       </c>
       <c r="Q19" s="4">
-        <v>338.40980251906001</v>
+        <v>621.225749845358</v>
       </c>
       <c r="R19" s="4">
-        <v>376.88403366249997</v>
+        <v>602.36943901751397</v>
       </c>
       <c r="S19" s="4">
-        <v>409.21203026410001</v>
+        <v>460.01323261444497</v>
       </c>
       <c r="T19" s="4">
-        <v>416.68556828014601</v>
+        <v>291.47438377357599</v>
       </c>
     </row>
     <row r="21" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>4.7355231636486401</v>
+        <v>1.1894452813260801</v>
       </c>
       <c r="B22" s="4">
-        <v>4.5169262005585296</v>
+        <v>1.1815604571759999</v>
       </c>
       <c r="C22" s="4">
-        <v>4.5087483273614799</v>
+        <v>1.1815604571759999</v>
       </c>
       <c r="D22" s="4">
-        <v>4.4561721166876396</v>
+        <v>1.1815604571759999</v>
       </c>
       <c r="E22" s="4">
-        <v>4.4561721166876396</v>
+        <v>1.12020649550942</v>
       </c>
       <c r="F22" s="4">
-        <v>4.4561721166876396</v>
+        <v>1.12020649550942</v>
       </c>
       <c r="G22" s="4">
-        <v>4.4463200627533501</v>
+        <v>1.12020649550942</v>
       </c>
       <c r="H22" s="4">
-        <v>4.4003247523462097</v>
+        <v>1.1073193065693301</v>
       </c>
       <c r="I22" s="4">
-        <v>4.2535850712239496</v>
+        <v>1.1073193065693301</v>
       </c>
       <c r="J22" s="4">
-        <v>4.2535850712239496</v>
+        <v>1.1073193065693301</v>
       </c>
       <c r="K22" s="4">
-        <v>4.2211028826571804</v>
+        <v>1.0920645100492501</v>
       </c>
       <c r="L22" s="4">
-        <v>4.19205506028465</v>
+        <v>1.0920645100492501</v>
       </c>
       <c r="M22" s="4">
-        <v>4.16332542025948</v>
+        <v>1.0864431657504601</v>
       </c>
       <c r="N22" s="4">
-        <v>4.1451378379639099</v>
+        <v>1.08571933826239</v>
       </c>
       <c r="O22" s="4">
-        <v>4.1261337677087804</v>
+        <v>1.08571933826239</v>
       </c>
       <c r="P22" s="4">
-        <v>4.0567348517525001</v>
+        <v>1.08571933826239</v>
       </c>
       <c r="Q22" s="4">
-        <v>4.0567348517525001</v>
+        <v>1.0446064012533001</v>
       </c>
       <c r="R22" s="4">
-        <v>4.0567348517525001</v>
+        <v>1.03181482991283</v>
       </c>
       <c r="S22" s="4">
-        <v>4.0351812066192903</v>
+        <v>1.03181482991283</v>
       </c>
       <c r="T22" s="4">
-        <v>4.0351812066192903</v>
+        <v>1.03181482991283</v>
       </c>
       <c r="U22" s="4">
-        <v>4.0351812066192903</v>
+        <v>1.03181482991283</v>
       </c>
       <c r="V22" s="4">
-        <v>4.0351812066192903</v>
+        <v>1.01875567651211</v>
       </c>
       <c r="W22" s="4">
-        <v>4.0351812066192903</v>
+        <v>0.91731545282295701</v>
       </c>
       <c r="X22" s="4">
-        <v>4.0351812066192903</v>
+        <v>0.91731545282295701</v>
       </c>
       <c r="Y22" s="4">
-        <v>4.0351812066192903</v>
+        <v>0.91731545282295701</v>
       </c>
       <c r="Z22" s="4">
-        <v>4.0351812066192903</v>
+        <v>0.863248380306887</v>
       </c>
       <c r="AA22" s="4">
-        <v>4.0351812066192903</v>
+        <v>0.863248380306887</v>
       </c>
       <c r="AB22" s="4">
-        <v>4.0351812066192903</v>
+        <v>0.863248380306887</v>
       </c>
       <c r="AC22" s="4">
-        <v>4.0351812066192903</v>
+        <v>0.863248380306887</v>
       </c>
       <c r="AD22" s="4">
-        <v>4.0271310249269101</v>
+        <v>0.863248380306887</v>
       </c>
       <c r="AE22" s="4">
-        <v>3.9718679070418701</v>
+        <v>0.81583993148976197</v>
       </c>
       <c r="AF22" s="4">
-        <v>3.9718679070418701</v>
+        <v>0.81583993148976197</v>
       </c>
       <c r="AG22" s="4">
-        <v>3.9718679070418701</v>
+        <v>0.799869425022812</v>
       </c>
       <c r="AH22" s="4">
-        <v>3.9718679070418701</v>
+        <v>0.653961108610978</v>
       </c>
       <c r="AI22" s="4">
-        <v>3.9718679070418701</v>
+        <v>0.653961108610978</v>
       </c>
       <c r="AJ22" s="4">
-        <v>3.9450687021033999</v>
+        <v>0.653961108610978</v>
       </c>
       <c r="AK22" s="4">
-        <v>3.9450687021033999</v>
+        <v>0.39355247977483199</v>
       </c>
       <c r="AL22" s="4">
-        <v>3.9450687021033999</v>
+        <v>0.291902838269197</v>
       </c>
       <c r="AM22" s="4">
-        <v>3.9450687021033999</v>
+        <v>0.291902838269197</v>
       </c>
       <c r="AN22" s="4">
-        <v>3.9450687021033999</v>
+        <v>0.291902838269197</v>
       </c>
       <c r="AO22" s="4">
-        <v>3.9450687021033999</v>
+        <v>0.291902838269197</v>
       </c>
       <c r="AP22" s="4">
-        <v>3.9450687021033999</v>
+        <v>0.291902838269197</v>
       </c>
       <c r="AQ22" s="4">
-        <v>3.9450687021033999</v>
+        <v>0.291902838269197</v>
       </c>
       <c r="AR22" s="4">
-        <v>3.9450687021033999</v>
+        <v>0.291902838269197</v>
       </c>
       <c r="AS22" s="4">
-        <v>3.91927952141591</v>
+        <v>0.21102837617776499</v>
       </c>
       <c r="AT22" s="4">
-        <v>3.91927952141591</v>
+        <v>0.21102837617776499</v>
       </c>
       <c r="AU22" s="4">
-        <v>3.91927952141591</v>
+        <v>0.20069866372822001</v>
       </c>
       <c r="AV22" s="4">
-        <v>3.91927952141591</v>
+        <v>0.20069866372822001</v>
       </c>
       <c r="AW22" s="4">
-        <v>3.91927952141591</v>
+        <v>0.20069866372822001</v>
       </c>
       <c r="AX22" s="4">
-        <v>3.91927952141591</v>
+        <v>0.19988263346424301</v>
       </c>
       <c r="AY22" s="4">
-        <v>3.91927952141591</v>
+        <v>0.19988263346424301</v>
       </c>
       <c r="AZ22" s="4">
-        <v>3.9071661887718001</v>
+        <v>1.10156213183784E-2</v>
       </c>
       <c r="BA22" s="4">
-        <v>3.9071661887718001</v>
+        <v>1.10156213183784E-2</v>
       </c>
       <c r="BB22" s="4">
-        <v>3.9071661887718001</v>
+        <v>1.10156213183784E-2</v>
       </c>
       <c r="BC22" s="4">
-        <v>3.9071661887718001</v>
+        <v>1.10156213183784E-2</v>
       </c>
       <c r="BD22" s="4">
-        <v>3.9071661887718001</v>
+        <v>-2.94700396696948E-2</v>
       </c>
       <c r="BE22" s="4">
-        <v>3.9071661887718001</v>
+        <v>-3.7623538004289601E-2</v>
       </c>
       <c r="BF22" s="4">
-        <v>3.9071661887718001</v>
+        <v>-3.7623538004289601E-2</v>
       </c>
       <c r="BG22" s="4">
-        <v>3.8827436025596</v>
+        <v>-3.7623538004289601E-2</v>
       </c>
       <c r="BH22" s="4">
-        <v>3.8827436025596</v>
+        <v>-3.7623538004289601E-2</v>
       </c>
       <c r="BI22" s="4">
-        <v>3.8827436025596</v>
+        <v>-3.7623538004289601E-2</v>
       </c>
       <c r="BJ22" s="4">
-        <v>3.8827436025596</v>
+        <v>-3.7623538004289601E-2</v>
       </c>
       <c r="BK22" s="4">
-        <v>3.8827436025596</v>
+        <v>-3.7623538004289601E-2</v>
       </c>
       <c r="BL22" s="4">
-        <v>3.8827436025596</v>
+        <v>-3.7623538004289601E-2</v>
       </c>
       <c r="BM22" s="4">
-        <v>3.8827436025596</v>
+        <v>-4.61925305490163E-2</v>
       </c>
       <c r="BN22" s="4">
-        <v>3.8827436025596</v>
+        <v>-4.61925305490163E-2</v>
       </c>
       <c r="BO22" s="4">
-        <v>3.8827436025596</v>
+        <v>-4.61925305490163E-2</v>
       </c>
       <c r="BP22" s="4">
-        <v>3.8827436025596</v>
+        <v>-4.61925305490163E-2</v>
       </c>
       <c r="BQ22" s="4">
-        <v>3.8827436025596</v>
+        <v>-4.61925305490163E-2</v>
       </c>
       <c r="BR22" s="4">
-        <v>3.8827436025596</v>
+        <v>-4.61925305490163E-2</v>
       </c>
       <c r="BS22" s="4">
-        <v>3.8827436025596</v>
+        <v>-4.61925305490163E-2</v>
       </c>
       <c r="BT22" s="4">
-        <v>3.8827436025596</v>
+        <v>-4.61925305490163E-2</v>
       </c>
       <c r="BU22" s="4">
-        <v>3.8827436025596</v>
+        <v>-4.61925305490163E-2</v>
       </c>
       <c r="BV22" s="4">
-        <v>3.8827436025596</v>
+        <v>-4.61925305490163E-2</v>
       </c>
       <c r="BW22" s="4">
-        <v>3.8827436025596</v>
+        <v>-4.61925305490163E-2</v>
       </c>
       <c r="BX22" s="4">
-        <v>3.8827436025596</v>
+        <v>-4.61925305490163E-2</v>
       </c>
       <c r="BY22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-4.8271169645900502E-2</v>
       </c>
       <c r="BZ22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-4.8271169645900502E-2</v>
       </c>
       <c r="CA22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-4.8271169645900502E-2</v>
       </c>
       <c r="CB22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-4.8271169645900502E-2</v>
       </c>
       <c r="CC22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-4.8271169645900502E-2</v>
       </c>
       <c r="CD22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-4.8271169645900502E-2</v>
       </c>
       <c r="CE22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-4.8271169645900502E-2</v>
       </c>
       <c r="CF22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-4.8271169645900502E-2</v>
       </c>
       <c r="CG22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-4.8271169645900502E-2</v>
       </c>
       <c r="CH22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-0.116083556860788</v>
       </c>
       <c r="CI22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-0.117258585137181</v>
       </c>
       <c r="CJ22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-0.13647503207598799</v>
       </c>
       <c r="CK22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-0.13647503207598799</v>
       </c>
       <c r="CL22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-0.13647503207598799</v>
       </c>
       <c r="CM22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-0.13647503207598799</v>
       </c>
       <c r="CN22" s="4">
-        <v>3.8617545089829401</v>
+        <v>-0.13647503207598799</v>
       </c>
       <c r="CO22" s="4">
-        <v>3.8600725704755501</v>
+        <v>-0.13647503207598799</v>
       </c>
       <c r="CP22" s="4">
-        <v>3.8600725704755501</v>
+        <v>-0.13647503207598799</v>
       </c>
       <c r="CQ22" s="4">
-        <v>3.8600725704755501</v>
+        <v>-0.13647503207598799</v>
       </c>
       <c r="CR22" s="4">
-        <v>3.8600725704755501</v>
+        <v>-0.13647503207598799</v>
       </c>
       <c r="CS22" s="4">
-        <v>3.8600725704755501</v>
+        <v>-0.13647503207598799</v>
       </c>
       <c r="CT22" s="4">
-        <v>3.8600725704755501</v>
+        <v>-0.13647503207598799</v>
       </c>
       <c r="CU22" s="4">
-        <v>3.8600725704755501</v>
+        <v>-0.13647503207598799</v>
       </c>
       <c r="CV22" s="4">
-        <v>3.8594679994154202</v>
+        <v>-0.13647503207598799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>